<commit_message>
#36697 Fixed to show app menu in the lanes correctly #36696 Fixed BGAlpha range (0-254 to 0-255) #36696 Fixed BGAlpha descriptions in English
</commit_message>
<xml_diff>
--- a/実行時フォルダ/System/resources.xlsx
+++ b/実行時フォルダ/System/resources.xlsx
@@ -726,9 +726,9 @@
     <t xml:space="preserve">BGAlpha</t>
   </si>
   <si>
-    <t xml:space="preserve">The transparent degree for playing screen and wallpaper.\n
+    <t xml:space="preserve">The opaque degree for playing screen and wallpaper.\n
 \n
-0=no transparent, 255=completely transparency.</t>
+0=no opacity, 255=full opacity.</t>
   </si>
   <si>
     <t xml:space="preserve">背景画像の透明割合：\n
@@ -4579,21 +4579,20 @@
   </sheetPr>
   <dimension ref="A1:G269"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.2613636363636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.9545454545455"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="171.528409090909"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.7670454545455"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.9772727272727"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="138.306818181818"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="60.4318181818182"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.8011363636364"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6818181818182"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="81.7784090909091"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.7670454545455"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="76.5284090909091"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6193181818182"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4318181818182"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="152.284090909091"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="66.4488636363636"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.3068181818182"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5096,7 +5095,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>136</v>
       </c>
@@ -7945,8 +7944,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.1534090909091"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.4261363636364"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.8125"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.4772727272727"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>